<commit_message>
Fulcrum images and text updates
</commit_message>
<xml_diff>
--- a/tables/Survey123_app_criteria2.xlsx
+++ b/tables/Survey123_app_criteria2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KAlstad\Documents\Github_C\e-device2\criteria_tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KAlstad\Documents\Github_C\e-device2\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{765E1527-5F9A-4AF7-91F5-EBFBCF5D4040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E26C639-61E8-4E0B-9CBA-90F291A09AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16500" windowWidth="29040" windowHeight="15840" xr2:uid="{E4A5BE10-DBB8-481B-874B-1BDF43DE8625}"/>
+    <workbookView xWindow="30810" yWindow="2655" windowWidth="24270" windowHeight="11385" activeTab="1" xr2:uid="{E4A5BE10-DBB8-481B-874B-1BDF43DE8625}"/>
   </bookViews>
   <sheets>
     <sheet name="Forms_Options" sheetId="1" r:id="rId1"/>
@@ -625,9 +625,6 @@
     <t>Not easily done</t>
   </si>
   <si>
-    <t>In trial demo: User noted that it was not possible to view the full list of fish lengths, and it was not easy to edit responses ‘on-the-fly’) (Appendix: 3)</t>
-  </si>
-  <si>
     <t>Can be downloaded as .CSV; User selects output format (CSV, Excel, KML, shapefile, or file geodatabase) </t>
   </si>
   <si>
@@ -834,6 +831,9 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>In trial demo: User noted that it was not possible to view the full list of fish lengths, and it was not easy to edit responses ‘on-the-fly’) [See Yolo BiPass Survey123 Demo](#yoldem))</t>
   </si>
 </sst>
 </file>
@@ -1394,8 +1394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FEDC525-B77D-4397-8B91-1C5526620A5B}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="105" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1594,7 +1594,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>63</v>
@@ -1611,7 +1611,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>78</v>
@@ -1803,8 +1803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C0BCC4-86A1-4030-90CE-22D0CC9ADA23}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1846,7 +1846,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>63</v>
@@ -1870,10 +1870,10 @@
         <v>78</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>112</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>113</v>
       </c>
       <c r="F3" s="10"/>
     </row>
@@ -1882,16 +1882,16 @@
         <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1905,10 +1905,10 @@
         <v>101</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="F5" s="4"/>
     </row>
@@ -1923,11 +1923,11 @@
         <v>63</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G6" s="6"/>
     </row>
@@ -1939,16 +1939,16 @@
         <v>14</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>107</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="5"/>
@@ -1964,7 +1964,7 @@
         <v>63</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -1994,7 +1994,7 @@
         <v>78</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2050,7 +2050,7 @@
         <v>63</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="5" customFormat="1" ht="254.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2064,7 +2064,7 @@
         <v>63</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2078,7 +2078,7 @@
         <v>63</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2092,10 +2092,10 @@
         <v>63</v>
       </c>
       <c r="D5" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="24" t="s">
         <v>117</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -2109,10 +2109,10 @@
         <v>63</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -2127,7 +2127,7 @@
         <v>63</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
@@ -2224,7 +2224,7 @@
         <v>63</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
@@ -2240,7 +2240,7 @@
         <v>25</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2292,10 +2292,10 @@
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2306,10 +2306,10 @@
         <v>63</v>
       </c>
       <c r="C3" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>128</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -2318,7 +2318,7 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2329,7 +2329,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2338,10 +2338,10 @@
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>132</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2354,7 +2354,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2375,7 +2375,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>96</v>
@@ -2394,10 +2394,10 @@
         <v>52</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>135</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -2410,10 +2410,10 @@
         <v>52</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -2426,10 +2426,10 @@
         <v>52</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>139</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -2442,7 +2442,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -2456,7 +2456,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2470,12 +2470,12 @@
         <v>54</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>

</xml_diff>